<commit_message>
Remove CDATA from xls
</commit_message>
<xml_diff>
--- a/automation/sar_geschaeftsberichte/OGD-Metadaten_Geschaeftsberichte.xlsx
+++ b/automation/sar_geschaeftsberichte/OGD-Metadaten_Geschaeftsberichte.xlsx
@@ -1023,40 +1023,6 @@
     <t>Name der Datei im Archivkatalog</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;![CDATA[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Seit 1859 legt der Stadtrat mit dem jährlich erscheinenden Geschäftsbericht der Gemeinde Rechenschaft über seine Tätigkeit ab.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]]&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>Archivische Verzeichnung</t>
   </si>
   <si>
@@ -1066,46 +1032,16 @@
     <t>geschaeftsbericht, stadtrat, archiv, archivdaten, geschichte, glam, openglam</t>
   </si>
   <si>
-    <t>&lt;![CDATA[
-Die Geschäftsberichte liegen als PDF vor und lassen sich Durchsuchen. Der Text wurde mittels OCR («Optical Character Recognition») extrahiert und ist in der Datei hinterlegt.
-]]&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;![CDATA[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Die [Geschäftsberichte](https://www.stadt-zuerich.ch/geschaeftsbericht) sind auch auf der Webseite der Stadt Zürich verfügbar. Dort können alle Geschäftsberichte im Volltext durchsucht werden.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]]&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>Stadtarchiv Zürich, Präsidialdepartement</t>
+  </si>
+  <si>
+    <t>Die Geschäftsberichte liegen als PDF vor und lassen sich Durchsuchen. Der Text wurde mittels OCR («Optical Character Recognition») extrahiert und ist in der Datei hinterlegt.</t>
+  </si>
+  <si>
+    <t>Seit 1859 legt der Stadtrat mit dem jährlich erscheinenden Geschäftsbericht der Gemeinde Rechenschaft über seine Tätigkeit ab.</t>
+  </si>
+  <si>
+    <t>Die [Geschäftsberichte](https://www.stadt-zuerich.ch/geschaeftsbericht) sind auch auf der Webseite der Stadt Zürich verfügbar. Dort können alle Geschäftsberichte im Volltext durchsucht werden.</t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1763,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1883,7 +1819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1894,7 +1830,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -1964,7 +1900,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
@@ -1982,7 +1918,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
@@ -2000,14 +1936,14 @@
         <v>14</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2104,7 +2040,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
@@ -2177,7 +2113,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -2185,7 +2121,7 @@
         <v>60</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
@@ -2265,7 +2201,7 @@
         <v>177</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="4" t="s">
@@ -3120,21 +3056,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3248,10 +3169,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3272,17 +3216,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>